<commit_message>
Final sentiment evaluation xcel
</commit_message>
<xml_diff>
--- a/sentiment analysis/sentiment model analysis.xlsx
+++ b/sentiment analysis/sentiment model analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\theis\Desktop\sentiment_analytics_exam\sentiment analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ED09394-84FA-490B-A141-4984CD0B99B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D29675A2-6C93-4289-BD23-7B874EC152C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{F19CB6AA-7F74-407D-9D54-B006C947AD37}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="44">
   <si>
     <t>zero-shot all-MiniLM-L6-v2</t>
   </si>
@@ -160,6 +160,15 @@
   </si>
   <si>
     <t>Label (Antagelse: Sentimentet er lavet ud fra om det er positivt eller negativt for aktien)</t>
+  </si>
+  <si>
+    <t>Final counts</t>
+  </si>
+  <si>
+    <t>Accuracy</t>
+  </si>
+  <si>
+    <t>Total cells</t>
   </si>
 </sst>
 </file>
@@ -534,10 +543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62238D87-CDB7-4237-9330-DBC8020B109B}">
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1255,6 +1264,78 @@
         <v>35</v>
       </c>
     </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>43</v>
+      </c>
+      <c r="B38" s="1">
+        <v>26</v>
+      </c>
+      <c r="C38" s="1">
+        <v>26</v>
+      </c>
+      <c r="D38" s="1">
+        <v>26</v>
+      </c>
+      <c r="E38" s="1">
+        <v>26</v>
+      </c>
+      <c r="F38" s="1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>41</v>
+      </c>
+      <c r="B39" s="1">
+        <v>7</v>
+      </c>
+      <c r="C39" s="1">
+        <v>21</v>
+      </c>
+      <c r="D39" s="1">
+        <v>9</v>
+      </c>
+      <c r="E39" s="1">
+        <v>11</v>
+      </c>
+      <c r="F39" s="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>42</v>
+      </c>
+      <c r="B41" s="1">
+        <f>B39/B38*100</f>
+        <v>26.923076923076923</v>
+      </c>
+      <c r="C41" s="1">
+        <f>C39/C38*100</f>
+        <v>80.769230769230774</v>
+      </c>
+      <c r="D41" s="1">
+        <f>D39/D38*100</f>
+        <v>34.615384615384613</v>
+      </c>
+      <c r="E41" s="1">
+        <f>E39/E38*100</f>
+        <v>42.307692307692307</v>
+      </c>
+      <c r="F41" s="1">
+        <f>F39/F38*100</f>
+        <v>80.769230769230774</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>